<commit_message>
WIP implement StationControler class
</commit_message>
<xml_diff>
--- a/Objectives.xlsx
+++ b/Objectives.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334B6B35-3481-43D8-BF59-7F7397CBA58A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BB6B28-ACFA-40BB-BCA6-3430241A8633}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Ref</t>
   </si>
@@ -51,13 +51,19 @@
     <t>Use Cartopy instead of BASEMAP</t>
   </si>
   <si>
-    <t>REF-GV-100</t>
-  </si>
-  <si>
     <t>DEV-GV-100</t>
   </si>
   <si>
     <t>Cartopy seems to be the rising star in term of cartography and display. Investigate possibility and effort to switch to cartopy if Basemap is abandonated. Also consider using only Pyproj and Matplotlib.</t>
+  </si>
+  <si>
+    <t>REV-GV-200</t>
+  </si>
+  <si>
+    <t>Implement inhibition of rectangular zoom trigger when taking focus over main windows.</t>
+  </si>
+  <si>
+    <t>REV-GV-100</t>
   </si>
 </sst>
 </file>
@@ -378,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -402,40 +408,51 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C5">
+    <sortCondition ref="A2:A5"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added tasks for development and debug to Objectives.xlsx
</commit_message>
<xml_diff>
--- a/Objectives.xlsx
+++ b/Objectives.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BB6B28-ACFA-40BB-BCA6-3430241A8633}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492B27A4-43F0-4A25-BBED-582B28A518F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Ref</t>
   </si>
@@ -64,6 +64,27 @@
   </si>
   <si>
     <t>REV-GV-100</t>
+  </si>
+  <si>
+    <t>REV-GV-300</t>
+  </si>
+  <si>
+    <t>Customisable slope range</t>
+  </si>
+  <si>
+    <t>implement customisable slope range in pattern widget</t>
+  </si>
+  <si>
+    <t>DEV-GV-300</t>
+  </si>
+  <si>
+    <t>DEV-GV-200</t>
+  </si>
+  <si>
+    <t>Extend pattern</t>
+  </si>
+  <si>
+    <t>opposite function to shrink pattern</t>
   </si>
 </sst>
 </file>
@@ -384,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,7 +442,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -447,6 +468,28 @@
       </c>
       <c r="B5" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create expand_copol. Factorized code with shrink_copol.
</commit_message>
<xml_diff>
--- a/Objectives.xlsx
+++ b/Objectives.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492B27A4-43F0-4A25-BBED-582B28A518F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFC6522-2299-4E22-BAC7-5F11FA9D51E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Ref</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>opposite function to shrink pattern</t>
+  </si>
+  <si>
+    <t>Val</t>
+  </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -405,20 +414,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.33203125" customWidth="1"/>
     <col min="3" max="3" width="84.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,8 +437,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -440,7 +452,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -451,7 +463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -462,7 +474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -470,7 +482,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -480,8 +492,11 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -490,6 +505,9 @@
       </c>
       <c r="C7" t="s">
         <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saved progress on Objectives.xlsx
</commit_message>
<xml_diff>
--- a/Objectives.xlsx
+++ b/Objectives.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFC6522-2299-4E22-BAC7-5F11FA9D51E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B45637-BD49-4C52-91F2-63D560785412}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Ref</t>
   </si>
@@ -90,10 +90,10 @@
     <t>Val</t>
   </si>
   <si>
-    <t>Dev</t>
-  </si>
-  <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Merged on DEV</t>
   </si>
 </sst>
 </file>
@@ -414,20 +414,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.33203125" customWidth="1"/>
     <col min="3" max="3" width="84.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,10 +438,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -452,7 +452,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -463,7 +463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -474,7 +474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -482,7 +482,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -496,7 +496,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -507,7 +507,10 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>